<commit_message>
time group in protocol
</commit_message>
<xml_diff>
--- a/protocol/FLs_protocol.xlsx
+++ b/protocol/FLs_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelperini/Documents/research/projects/Lsax_fertilisation_time/protocol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CD52E6-A061-AD4B-86A8-1B4E15C17ED0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E48A7D-1E13-454B-A2B2-DF1345316F84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="29340" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>FLs mating trials</t>
+  </si>
+  <si>
+    <t>Time group</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD40"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -863,7 +866,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -1002,7 +1007,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1141,7 +1148,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A27" s="8"/>
+      <c r="A27" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -1280,7 +1289,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1">
-      <c r="A38" s="12"/>
+      <c r="A38" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>

</xml_diff>

<commit_message>
minor changes to the protocol sheet
</commit_message>
<xml_diff>
--- a/protocol/FLs_protocol.xlsx
+++ b/protocol/FLs_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelperini/Documents/research/projects/Lsax_fertilisation_time/protocol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E48A7D-1E13-454B-A2B2-DF1345316F84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8D5582-B7ED-C247-9733-A3D463B3943C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="29340" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -242,19 +242,6 @@
       <right style="double">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
       <top style="double">
         <color auto="1"/>
       </top>
@@ -420,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,25 +418,24 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,43 +811,43 @@
     <row r="2" spans="1:7" ht="16" thickBot="1"/>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="5"/>
-      <c r="B3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -869,523 +855,523 @@
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="20"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="20"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="20"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="20"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="20"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="13" t="s">
+      <c r="B14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="13" t="s">
+      <c r="B15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="25"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="20"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1">
       <c r="A24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="20"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="13" t="s">
+      <c r="B25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="13" t="s">
+      <c r="B26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="25"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="20"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="20"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="20"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="20"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="20"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1">
       <c r="A35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="10"/>
-      <c r="B36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="13" t="s">
+      <c r="B36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A37" s="11"/>
-      <c r="B37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="13" t="s">
+      <c r="B37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="25"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="20"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="20"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="19"/>
     </row>
     <row r="42" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="20"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="20"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A45" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="20"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="20"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>